<commit_message>
cover with test & fix condition that check if current rendered cell was out of column amount limit (16384).
this test catch Exception and required a fix, becouse ExcelJS works on 1-based numeration but xlsx-render works on 0-indexed numeration (so here 16384 is equal to 16385 in ExcelJs)
</commit_message>
<xml_diff>
--- a/tests/integration/data/Renderer001-EndRow/expected.xlsx
+++ b/tests/integration/data/Renderer001-EndRow/expected.xlsx
@@ -1,37 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\siemi\aProjects\xlsx-renderer\tests\integration\data\Renderer001-EndRow\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DA2475BB-7C29-4976-82ED-5DAD3CE071ED}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="24580" windowHeight="14620" xr2:uid="{DA12C0B8-6741-444F-B263-55021EDA3A25}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="27795" windowHeight="16440" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet sheetId="1" name="Sheet1" state="visible" r:id="rId4"/>
+    <sheet sheetId="2" name="without EndRow" state="visible" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>#! FINISHED</t>
   </si>
@@ -43,33 +27,42 @@
   </si>
   <si>
     <t>C1 &amp; B2 should not been evaluated</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>#! FINISH</t>
+  </si>
+  <si>
+    <t>&lt;-- this `#! FINISH` should be in output, because the line above hasn't `END_ROW` that couse finish rendering on out of column limit reached (16384 columns)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="4">
@@ -99,19 +92,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Bad" xfId="1" builtinId="27"/>
-    <cellStyle name="Good" xfId="2" builtinId="26"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -423,43 +412,106 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BE5C9A7-554C-4824-A0F2-3EAE2478AA4A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.6328125" customWidth="1"/>
-    <col min="2" max="2" width="14.54296875" customWidth="1"/>
+    <col min="1" max="1" width="43.5703125" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="0" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:XFD3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>2</v>
+      </c>
+      <c r="C1">
+        <v>3</v>
+      </c>
+      <c r="D1">
+        <v>4</v>
+      </c>
+      <c r="E1">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16384" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>4</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
+      <c r="I2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>